<commit_message>
Add processing script for Remand Accused Details and update file paths
</commit_message>
<xml_diff>
--- a/Output/Processed.xlsx
+++ b/Output/Processed.xlsx
@@ -481,12 +481,12 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 9</t>
+          <t>2.PhoneNumber</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 10</t>
+          <t>3.PhoneNumber</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -534,26 +534,10 @@
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>2.PhoneNumber</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>3.PhoneNumber</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>185/24</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>303(2)BNS</t>
-        </is>
-      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -591,16 +575,8 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>282/24</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>8(c),20(b)(ii)(B),25,29(1)-NDPSACT</t>
-        </is>
-      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -638,16 +614,8 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>282/24</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>8(c),20(b)(ii)(B),25,29(1)-NDPSACT</t>
-        </is>
-      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -685,16 +653,8 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>282/24</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>8(c),20(b)(ii)(B),25,29(1)-NDPSACT</t>
-        </is>
-      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -732,16 +692,8 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>87/24</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>153,505(2)-IPC25(1A)-ARMSACT</t>
-        </is>
-      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -779,16 +731,8 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>246/24</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>24(1)COTPAct</t>
-        </is>
-      </c>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -826,16 +770,8 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>246/23</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>294(b),323,506(ii)IPC</t>
-        </is>
-      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -873,16 +809,8 @@
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>273/24</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>296(b),109(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -920,16 +848,8 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>271/24</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>296b,115(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1010,16 +930,8 @@
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>292/24</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>296(b),308(4),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1057,16 +969,8 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>70/2024</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>:296(b),309(4),351(3)BNSMOI(R)</t>
-        </is>
-      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1104,16 +1008,8 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>297/24</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>296(b),308(4),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1151,16 +1047,8 @@
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>422/24</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>4(1)(A)TNPACT</t>
-        </is>
-      </c>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1198,16 +1086,8 @@
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>194/24</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>296,115(2),118(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1245,16 +1125,8 @@
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>421/2024</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>3ofTNPPDLAct</t>
-        </is>
-      </c>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1292,16 +1164,8 @@
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>269/24</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>296(b),132,351(3)BNSAct(Technical)</t>
-        </is>
-      </c>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1347,16 +1211,8 @@
       </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>159/24</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>310(2)BNS</t>
-        </is>
-      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1417,16 +1273,8 @@
       </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>184/2024</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>.126(2),296(b),309(6),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1476,16 +1324,8 @@
         </is>
       </c>
       <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>86/2024</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>296(b),118(1),351(3)BNS&amp;92(a),92(e)THERIGHTSOFPERSONwithDISABILITIESAct2016</t>
-        </is>
-      </c>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1535,16 +1375,8 @@
       </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>22/24</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>303(2)BNS</t>
-        </is>
-      </c>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1648,16 +1480,8 @@
       </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>251/24</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>296(b),118(1),351(3)-BNS</t>
-        </is>
-      </c>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1703,16 +1527,8 @@
       </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>389/24</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>269BNS</t>
-        </is>
-      </c>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1762,16 +1578,8 @@
       </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>478/24</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>331(3),331(4),305BNS(HBNight)</t>
-        </is>
-      </c>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1819,16 +1627,8 @@
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>278/2024</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>.126(2),296(b),308(4),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1874,16 +1674,8 @@
       </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>130/24</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>296(b),115(ii)118,351(3)BNSand4ofTNPHWAct</t>
-        </is>
-      </c>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1939,18 +1731,10 @@
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>427/2024</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>.
-329,296(b),
-351(3)BNSand
-4ofTNPWHActand
-3ofTNPPDLAct</t>
-        </is>
-      </c>
+          <t>427/2024/329296351343</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2020,16 +1804,8 @@
       </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>428/2024</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>296(b)311351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2081,16 +1857,8 @@
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>11/24</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>.3(a),4,9(l),9(m),9(n),10ofPocsoAct</t>
-        </is>
-      </c>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2143,16 +1911,8 @@
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>250/24</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>296(b),132,351(3),303(2)BNS</t>
-        </is>
-      </c>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2198,16 +1958,8 @@
       </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>173/24</t>
-        </is>
-      </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>379IPC(SandTheft)</t>
-        </is>
-      </c>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2253,16 +2005,8 @@
       </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>190/24</t>
-        </is>
-      </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>379IPC(SandTheft)</t>
-        </is>
-      </c>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2312,16 +2056,8 @@
       </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>132/2024</t>
-        </is>
-      </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>309(4)-BNS</t>
-        </is>
-      </c>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2418,16 +2154,8 @@
       </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>285/2024</t>
-        </is>
-      </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>331(4),305,62-BNS</t>
-        </is>
-      </c>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2481,16 +2209,8 @@
           <t>3)8072546793</t>
         </is>
       </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>394/24</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>296(b,132,351(3)BNSand24(1)COTPAAct</t>
-        </is>
-      </c>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2536,16 +2256,8 @@
       </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>394/24</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>296(b,132,351(3)BNSand24(1)COTPAAct</t>
-        </is>
-      </c>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2591,16 +2303,8 @@
       </c>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr"/>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>482/24</t>
-        </is>
-      </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>296(b),118(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2646,16 +2350,8 @@
       </c>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>486/24</t>
-        </is>
-      </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>296(b),118(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2701,16 +2397,8 @@
       </c>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>152/24</t>
-        </is>
-      </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>305BNS</t>
-        </is>
-      </c>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2756,16 +2444,8 @@
       </c>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>152/24</t>
-        </is>
-      </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>305BNS</t>
-        </is>
-      </c>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2811,16 +2491,8 @@
       </c>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>152/24</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>305BNS</t>
-        </is>
-      </c>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2917,16 +2589,8 @@
       </c>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>11/2024</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>417,376IPC</t>
-        </is>
-      </c>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2968,16 +2632,8 @@
       </c>
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr"/>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>426/24</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>8(c)r/w20(b)(ii)(B)NDPSAct</t>
-        </is>
-      </c>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -3076,16 +2732,8 @@
         </is>
       </c>
       <c r="K49" t="inlineStr"/>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>188/24</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>296(b),109,351(3),49-BNS</t>
-        </is>
-      </c>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3131,16 +2779,8 @@
       </c>
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr"/>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>209/24</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>8(c),20(b),(ii)(A)NDPSActand296(b),132,351(3),BNS</t>
-        </is>
-      </c>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3186,16 +2826,8 @@
       </c>
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr"/>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>435/2024</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>296(b),118(i),351(3)BNSAct</t>
-        </is>
-      </c>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -3241,16 +2873,8 @@
       </c>
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="inlineStr"/>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>487/24</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>296(b),308(2),115(2),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3298,16 +2922,8 @@
       </c>
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="inlineStr"/>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>487/24</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>296(b),308(2),115(2),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3353,16 +2969,8 @@
       </c>
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr"/>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>487/24</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>296(b),308(2),115(2),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3408,16 +3016,8 @@
       </c>
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr"/>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>434/2024</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>296(b),118(i),351(3)BNSAct</t>
-        </is>
-      </c>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3463,16 +3063,8 @@
       </c>
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="inlineStr"/>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>435/2024</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>296(b),118(i),351(3)BNSAct</t>
-        </is>
-      </c>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3518,16 +3110,8 @@
       </c>
       <c r="J57" t="inlineStr"/>
       <c r="K57" t="inlineStr"/>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>75/21</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>394,392IPC</t>
-        </is>
-      </c>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3569,16 +3153,8 @@
       <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr"/>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>224/2024</t>
-        </is>
-      </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>7(1)LotteriesRegulationAct</t>
-        </is>
-      </c>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3620,16 +3196,8 @@
       <c r="I59" t="inlineStr"/>
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="inlineStr"/>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>163/24</t>
-        </is>
-      </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>305BNS</t>
-        </is>
-      </c>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3677,16 +3245,8 @@
       <c r="I60" t="inlineStr"/>
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="inlineStr"/>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>192/2024</t>
-        </is>
-      </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>:296(b),109,351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3734,16 +3294,8 @@
       </c>
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>287/24</t>
-        </is>
-      </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>191(2),191(3),126(2),127(2),296(b),118(1),109,351(3)-BNS</t>
-        </is>
-      </c>
+      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3791,16 +3343,8 @@
       </c>
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr"/>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>287/24</t>
-        </is>
-      </c>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>191(2),191(3),126(2),127(2),296(b),118(1),109,351(3)-BNS</t>
-        </is>
-      </c>
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3846,16 +3390,8 @@
       </c>
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="inlineStr"/>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>287/24</t>
-        </is>
-      </c>
-      <c r="M63" t="inlineStr">
-        <is>
-          <t>191(2),191(3),126(2),127(2),296(b),118(1),109,351(3)-BNS</t>
-        </is>
-      </c>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3903,16 +3439,8 @@
       </c>
       <c r="J64" t="inlineStr"/>
       <c r="K64" t="inlineStr"/>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>287/24</t>
-        </is>
-      </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>191(2),191(3),126(2),127(2),296(b),118(1),109,351(3)-BNS</t>
-        </is>
-      </c>
+      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3958,16 +3486,8 @@
       </c>
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="inlineStr"/>
-      <c r="L65" t="inlineStr">
-        <is>
-          <t>287/24</t>
-        </is>
-      </c>
-      <c r="M65" t="inlineStr">
-        <is>
-          <t>191(2),191(3),126(2),127(2),296(b),118(1),109,351(3)-BNS</t>
-        </is>
-      </c>
+      <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -4009,16 +3529,8 @@
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="inlineStr"/>
-      <c r="L66" t="inlineStr">
-        <is>
-          <t>399/24</t>
-        </is>
-      </c>
-      <c r="M66" t="inlineStr">
-        <is>
-          <t>126(2),296(b),131,351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -4060,16 +3572,8 @@
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="inlineStr"/>
-      <c r="L67" t="inlineStr">
-        <is>
-          <t>399/24</t>
-        </is>
-      </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>126(2),296(b),131,351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -4111,16 +3615,8 @@
       <c r="I68" t="inlineStr"/>
       <c r="J68" t="inlineStr"/>
       <c r="K68" t="inlineStr"/>
-      <c r="L68" t="inlineStr">
-        <is>
-          <t>399/24</t>
-        </is>
-      </c>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>126(2),296(b),131,351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -4164,16 +3660,8 @@
       <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr"/>
       <c r="K69" t="inlineStr"/>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>400/24</t>
-        </is>
-      </c>
-      <c r="M69" t="inlineStr">
-        <is>
-          <t>296(b),115(2),74,76,109(1),351(3)BNSand4ofTNPHWAct</t>
-        </is>
-      </c>
+      <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -4217,16 +3705,8 @@
       <c r="I70" t="inlineStr"/>
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr"/>
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>401/24</t>
-        </is>
-      </c>
-      <c r="M70" t="inlineStr">
-        <is>
-          <t>132,351(3)BNSand4ofTNPHWAct</t>
-        </is>
-      </c>
+      <c r="L70" t="inlineStr"/>
+      <c r="M70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -4272,16 +3752,8 @@
       </c>
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr"/>
-      <c r="L71" t="inlineStr">
-        <is>
-          <t>441/2024</t>
-        </is>
-      </c>
-      <c r="M71" t="inlineStr">
-        <is>
-          <t>304(2)BNS</t>
-        </is>
-      </c>
+      <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -4325,16 +3797,8 @@
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr"/>
-      <c r="L72" t="inlineStr">
-        <is>
-          <t>441/2024</t>
-        </is>
-      </c>
-      <c r="M72" t="inlineStr">
-        <is>
-          <t>304(2)BNS</t>
-        </is>
-      </c>
+      <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -4380,16 +3844,8 @@
       </c>
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr"/>
-      <c r="L73" t="inlineStr">
-        <is>
-          <t>441/2024</t>
-        </is>
-      </c>
-      <c r="M73" t="inlineStr">
-        <is>
-          <t>304(2)BNS</t>
-        </is>
-      </c>
+      <c r="L73" t="inlineStr"/>
+      <c r="M73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -4435,16 +3891,8 @@
       </c>
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr"/>
-      <c r="L74" t="inlineStr">
-        <is>
-          <t>441/2024</t>
-        </is>
-      </c>
-      <c r="M74" t="inlineStr">
-        <is>
-          <t>304(2)BNS</t>
-        </is>
-      </c>
+      <c r="L74" t="inlineStr"/>
+      <c r="M74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -4490,16 +3938,8 @@
       </c>
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr"/>
-      <c r="L75" t="inlineStr">
-        <is>
-          <t>442/2024</t>
-        </is>
-      </c>
-      <c r="M75" t="inlineStr">
-        <is>
-          <t>126(2),296(b),311,351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L75" t="inlineStr"/>
+      <c r="M75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4545,16 +3985,8 @@
       </c>
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr"/>
-      <c r="L76" t="inlineStr">
-        <is>
-          <t>442/2024</t>
-        </is>
-      </c>
-      <c r="M76" t="inlineStr">
-        <is>
-          <t>126(2),296(b),311,351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L76" t="inlineStr"/>
+      <c r="M76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4602,16 +4034,8 @@
       </c>
       <c r="J77" t="inlineStr"/>
       <c r="K77" t="inlineStr"/>
-      <c r="L77" t="inlineStr">
-        <is>
-          <t>130/11</t>
-        </is>
-      </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>457,380IPC</t>
-        </is>
-      </c>
+      <c r="L77" t="inlineStr"/>
+      <c r="M77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -4657,16 +4081,8 @@
       </c>
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="inlineStr"/>
-      <c r="L78" t="inlineStr">
-        <is>
-          <t>13/24</t>
-        </is>
-      </c>
-      <c r="M78" t="inlineStr">
-        <is>
-          <t>417,376,506(ii)IPC</t>
-        </is>
-      </c>
+      <c r="L78" t="inlineStr"/>
+      <c r="M78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4708,16 +4124,8 @@
       </c>
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr"/>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>288/24</t>
-        </is>
-      </c>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>191(2),191(3),296(b),115(2),118(1),324(4),351(3)-BNS</t>
-        </is>
-      </c>
+      <c r="L79" t="inlineStr"/>
+      <c r="M79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -4763,16 +4171,8 @@
       </c>
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="inlineStr"/>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>288/24</t>
-        </is>
-      </c>
-      <c r="M80" t="inlineStr">
-        <is>
-          <t>191(2),191(3),296(b),115(2),118(1),324(4),351(3)-BNS</t>
-        </is>
-      </c>
+      <c r="L80" t="inlineStr"/>
+      <c r="M80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -4822,16 +4222,8 @@
       </c>
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr"/>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>78/2024</t>
-        </is>
-      </c>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>331(4),62BNS</t>
-        </is>
-      </c>
+      <c r="L81" t="inlineStr"/>
+      <c r="M81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -4877,16 +4269,8 @@
       </c>
       <c r="J82" t="inlineStr"/>
       <c r="K82" t="inlineStr"/>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>211/24</t>
-        </is>
-      </c>
-      <c r="M82" t="inlineStr">
-        <is>
-          <t>133,296(b),118910,351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L82" t="inlineStr"/>
+      <c r="M82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -4935,16 +4319,8 @@
       </c>
       <c r="J83" t="inlineStr"/>
       <c r="K83" t="inlineStr"/>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>255/24</t>
-        </is>
-      </c>
-      <c r="M83" t="inlineStr">
-        <is>
-          <t>303(2)BNS</t>
-        </is>
-      </c>
+      <c r="L83" t="inlineStr"/>
+      <c r="M83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -4998,16 +4374,8 @@
       </c>
       <c r="J84" t="inlineStr"/>
       <c r="K84" t="inlineStr"/>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>188/24</t>
-        </is>
-      </c>
-      <c r="M84" t="inlineStr">
-        <is>
-          <t>191(2),296(2),109,351(3),49,249BNS</t>
-        </is>
-      </c>
+      <c r="L84" t="inlineStr"/>
+      <c r="M84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -5053,16 +4421,8 @@
       </c>
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="inlineStr"/>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>404/24</t>
-        </is>
-      </c>
-      <c r="M85" t="inlineStr">
-        <is>
-          <t>303(2)BNSand21(1)minesandMinaralAct</t>
-        </is>
-      </c>
+      <c r="L85" t="inlineStr"/>
+      <c r="M85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -5108,16 +4468,8 @@
       </c>
       <c r="J86" t="inlineStr"/>
       <c r="K86" t="inlineStr"/>
-      <c r="L86" t="inlineStr">
-        <is>
-          <t>404/24</t>
-        </is>
-      </c>
-      <c r="M86" t="inlineStr">
-        <is>
-          <t>303(2)BNSand21(1)minesandMinaralAct</t>
-        </is>
-      </c>
+      <c r="L86" t="inlineStr"/>
+      <c r="M86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -5183,16 +4535,8 @@
       </c>
       <c r="J87" t="inlineStr"/>
       <c r="K87" t="inlineStr"/>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>88/2024</t>
-        </is>
-      </c>
-      <c r="M87" t="inlineStr">
-        <is>
-          <t>296(b),132,351(3)BNS&amp;8(c)r/w20(b)(ii)(A)NDPSAct1985</t>
-        </is>
-      </c>
+      <c r="L87" t="inlineStr"/>
+      <c r="M87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -5267,16 +4611,8 @@
       </c>
       <c r="J88" t="inlineStr"/>
       <c r="K88" t="inlineStr"/>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>447/2024</t>
-        </is>
-      </c>
-      <c r="M88" t="inlineStr">
-        <is>
-          <t>303(2)BNS</t>
-        </is>
-      </c>
+      <c r="L88" t="inlineStr"/>
+      <c r="M88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -5332,16 +4668,8 @@
       </c>
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr"/>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>447/2024</t>
-        </is>
-      </c>
-      <c r="M89" t="inlineStr">
-        <is>
-          <t>303(2)BNS</t>
-        </is>
-      </c>
+      <c r="L89" t="inlineStr"/>
+      <c r="M89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -5387,16 +4715,8 @@
       </c>
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="inlineStr"/>
-      <c r="L90" t="inlineStr">
-        <is>
-          <t>302/2024</t>
-        </is>
-      </c>
-      <c r="M90" t="inlineStr">
-        <is>
-          <t>:75(2)BNS&amp;4ofTNWHACT</t>
-        </is>
-      </c>
+      <c r="L90" t="inlineStr"/>
+      <c r="M90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -5438,16 +4758,8 @@
       </c>
       <c r="J91" t="inlineStr"/>
       <c r="K91" t="inlineStr"/>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>180/24</t>
-        </is>
-      </c>
-      <c r="M91" t="inlineStr">
-        <is>
-          <t>7,8,16,17,POCSOAct&amp;115(2)BNS</t>
-        </is>
-      </c>
+      <c r="L91" t="inlineStr"/>
+      <c r="M91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -5489,16 +4801,8 @@
       </c>
       <c r="J92" t="inlineStr"/>
       <c r="K92" t="inlineStr"/>
-      <c r="L92" t="inlineStr">
-        <is>
-          <t>180/24</t>
-        </is>
-      </c>
-      <c r="M92" t="inlineStr">
-        <is>
-          <t>7,8,16,17,POCSOAct&amp;115(2)BNS</t>
-        </is>
-      </c>
+      <c r="L92" t="inlineStr"/>
+      <c r="M92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -5570,16 +4874,8 @@
       </c>
       <c r="J93" t="inlineStr"/>
       <c r="K93" t="inlineStr"/>
-      <c r="L93" t="inlineStr">
-        <is>
-          <t>256/2024</t>
-        </is>
-      </c>
-      <c r="M93" t="inlineStr">
-        <is>
-          <t>.8(c)r/w.20(b)(ii)(A)NDPSAct&amp;Sec.77ofJJAct</t>
-        </is>
-      </c>
+      <c r="L93" t="inlineStr"/>
+      <c r="M93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -5629,16 +4925,8 @@
       </c>
       <c r="J94" t="inlineStr"/>
       <c r="K94" t="inlineStr"/>
-      <c r="L94" t="inlineStr">
-        <is>
-          <t>256/2024</t>
-        </is>
-      </c>
-      <c r="M94" t="inlineStr">
-        <is>
-          <t>.8(c)r/w.20(b)(ii)(A)NDPSAct&amp;Sec.77ofJJAct</t>
-        </is>
-      </c>
+      <c r="L94" t="inlineStr"/>
+      <c r="M94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -5691,16 +4979,8 @@
       </c>
       <c r="J95" t="inlineStr"/>
       <c r="K95" t="inlineStr"/>
-      <c r="L95" t="inlineStr">
-        <is>
-          <t>163/2024</t>
-        </is>
-      </c>
-      <c r="M95" t="inlineStr">
-        <is>
-          <t>296(b),351(3)BNS&amp;25(1A)ArmsAct</t>
-        </is>
-      </c>
+      <c r="L95" t="inlineStr"/>
+      <c r="M95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -5755,16 +5035,8 @@
       </c>
       <c r="J96" t="inlineStr"/>
       <c r="K96" t="inlineStr"/>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>163/2024</t>
-        </is>
-      </c>
-      <c r="M96" t="inlineStr">
-        <is>
-          <t>296(b),351(3)BNS&amp;25(1A)ArmsAct</t>
-        </is>
-      </c>
+      <c r="L96" t="inlineStr"/>
+      <c r="M96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -5818,16 +5090,8 @@
       </c>
       <c r="J97" t="inlineStr"/>
       <c r="K97" t="inlineStr"/>
-      <c r="L97" t="inlineStr">
-        <is>
-          <t>57/24</t>
-        </is>
-      </c>
-      <c r="M97" t="inlineStr">
-        <is>
-          <t>.296(b),115(2),331(2),74,75,76,351(2)BNS&amp;4ofTNPHWAcr</t>
-        </is>
-      </c>
+      <c r="L97" t="inlineStr"/>
+      <c r="M97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -5878,16 +5142,8 @@
       </c>
       <c r="J98" t="inlineStr"/>
       <c r="K98" t="inlineStr"/>
-      <c r="L98" t="inlineStr">
-        <is>
-          <t>295/2024</t>
-        </is>
-      </c>
-      <c r="M98" t="inlineStr">
-        <is>
-          <t>304BNS</t>
-        </is>
-      </c>
+      <c r="L98" t="inlineStr"/>
+      <c r="M98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -5959,16 +5215,8 @@
         </is>
       </c>
       <c r="K99" t="inlineStr"/>
-      <c r="L99" t="inlineStr">
-        <is>
-          <t>194/24</t>
-        </is>
-      </c>
-      <c r="M99" t="inlineStr">
-        <is>
-          <t>303(2)BNS</t>
-        </is>
-      </c>
+      <c r="L99" t="inlineStr"/>
+      <c r="M99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -6020,16 +5268,8 @@
       </c>
       <c r="J100" t="inlineStr"/>
       <c r="K100" t="inlineStr"/>
-      <c r="L100" t="inlineStr">
-        <is>
-          <t>194/24</t>
-        </is>
-      </c>
-      <c r="M100" t="inlineStr">
-        <is>
-          <t>303(2)BNS</t>
-        </is>
-      </c>
+      <c r="L100" t="inlineStr"/>
+      <c r="M100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -6082,16 +5322,8 @@
       </c>
       <c r="J101" t="inlineStr"/>
       <c r="K101" t="inlineStr"/>
-      <c r="L101" t="inlineStr">
-        <is>
-          <t>434/2024</t>
-        </is>
-      </c>
-      <c r="M101" t="inlineStr">
-        <is>
-          <t>296(b),118(i),351(3)BNSAct</t>
-        </is>
-      </c>
+      <c r="L101" t="inlineStr"/>
+      <c r="M101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -6129,16 +5361,8 @@
       <c r="I102" t="inlineStr"/>
       <c r="J102" t="inlineStr"/>
       <c r="K102" t="inlineStr"/>
-      <c r="L102" t="inlineStr">
-        <is>
-          <t>426/24</t>
-        </is>
-      </c>
-      <c r="M102" t="inlineStr">
-        <is>
-          <t>8(c)r/w20(b)(ii)(B)NDPSACT</t>
-        </is>
-      </c>
+      <c r="L102" t="inlineStr"/>
+      <c r="M102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -6182,16 +5406,8 @@
       </c>
       <c r="J103" t="inlineStr"/>
       <c r="K103" t="inlineStr"/>
-      <c r="L103" t="inlineStr">
-        <is>
-          <t>502/24</t>
-        </is>
-      </c>
-      <c r="M103" t="inlineStr">
-        <is>
-          <t>296(b),115(2),118(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L103" t="inlineStr"/>
+      <c r="M103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -6233,16 +5449,8 @@
       <c r="I104" t="inlineStr"/>
       <c r="J104" t="inlineStr"/>
       <c r="K104" t="inlineStr"/>
-      <c r="L104" t="inlineStr">
-        <is>
-          <t>502/24</t>
-        </is>
-      </c>
-      <c r="M104" t="inlineStr">
-        <is>
-          <t>296(b),115(2),118(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L104" t="inlineStr"/>
+      <c r="M104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -6286,16 +5494,8 @@
       </c>
       <c r="J105" t="inlineStr"/>
       <c r="K105" t="inlineStr"/>
-      <c r="L105" t="inlineStr">
-        <is>
-          <t>502/24</t>
-        </is>
-      </c>
-      <c r="M105" t="inlineStr">
-        <is>
-          <t>296(b),115(2),118(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L105" t="inlineStr"/>
+      <c r="M105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -6337,16 +5537,8 @@
       <c r="I106" t="inlineStr"/>
       <c r="J106" t="inlineStr"/>
       <c r="K106" t="inlineStr"/>
-      <c r="L106" t="inlineStr">
-        <is>
-          <t>503/24</t>
-        </is>
-      </c>
-      <c r="M106" t="inlineStr">
-        <is>
-          <t>296(b),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L106" t="inlineStr"/>
+      <c r="M106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -6388,16 +5580,8 @@
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr"/>
       <c r="K107" t="inlineStr"/>
-      <c r="L107" t="inlineStr">
-        <is>
-          <t>504/24</t>
-        </is>
-      </c>
-      <c r="M107" t="inlineStr">
-        <is>
-          <t>296(b),115,118(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L107" t="inlineStr"/>
+      <c r="M107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -6444,16 +5628,8 @@
       </c>
       <c r="J108" t="inlineStr"/>
       <c r="K108" t="inlineStr"/>
-      <c r="L108" t="inlineStr">
-        <is>
-          <t>262/2024</t>
-        </is>
-      </c>
-      <c r="M108" t="inlineStr">
-        <is>
-          <t>:126(2),296(b),308(4),351(3)BNSAct</t>
-        </is>
-      </c>
+      <c r="L108" t="inlineStr"/>
+      <c r="M108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -6721,16 +5897,8 @@
       <c r="I112" t="inlineStr"/>
       <c r="J112" t="inlineStr"/>
       <c r="K112" t="inlineStr"/>
-      <c r="L112" t="inlineStr">
-        <is>
-          <t>429/24</t>
-        </is>
-      </c>
-      <c r="M112" t="inlineStr">
-        <is>
-          <t>8©r/w20(b)(ii)(B)29(i)25NDPSACT</t>
-        </is>
-      </c>
+      <c r="L112" t="inlineStr"/>
+      <c r="M112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -6772,16 +5940,8 @@
       <c r="I113" t="inlineStr"/>
       <c r="J113" t="inlineStr"/>
       <c r="K113" t="inlineStr"/>
-      <c r="L113" t="inlineStr">
-        <is>
-          <t>429/24</t>
-        </is>
-      </c>
-      <c r="M113" t="inlineStr">
-        <is>
-          <t>8©r/w20(b)(ii)(B)29(i)25NDPSACT</t>
-        </is>
-      </c>
+      <c r="L113" t="inlineStr"/>
+      <c r="M113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -6823,16 +5983,8 @@
       <c r="I114" t="inlineStr"/>
       <c r="J114" t="inlineStr"/>
       <c r="K114" t="inlineStr"/>
-      <c r="L114" t="inlineStr">
-        <is>
-          <t>429/24</t>
-        </is>
-      </c>
-      <c r="M114" t="inlineStr">
-        <is>
-          <t>8©r/w20(b)(ii)(B)29(i)25NDPSACT</t>
-        </is>
-      </c>
+      <c r="L114" t="inlineStr"/>
+      <c r="M114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -6888,16 +6040,8 @@
       </c>
       <c r="J115" t="inlineStr"/>
       <c r="K115" t="inlineStr"/>
-      <c r="L115" t="inlineStr">
-        <is>
-          <t>506/24</t>
-        </is>
-      </c>
-      <c r="M115" t="inlineStr">
-        <is>
-          <t>105BNS</t>
-        </is>
-      </c>
+      <c r="L115" t="inlineStr"/>
+      <c r="M115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -6944,16 +6088,8 @@
       </c>
       <c r="J116" t="inlineStr"/>
       <c r="K116" t="inlineStr"/>
-      <c r="L116" t="inlineStr">
-        <is>
-          <t>126/2024</t>
-        </is>
-      </c>
-      <c r="M116" t="inlineStr">
-        <is>
-          <t>.296(b),115(2),351(3),303(2)(NP)BNS&amp;4OFTNPHWACT</t>
-        </is>
-      </c>
+      <c r="L116" t="inlineStr"/>
+      <c r="M116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -7113,16 +6249,8 @@
       <c r="I119" t="inlineStr"/>
       <c r="J119" t="inlineStr"/>
       <c r="K119" t="inlineStr"/>
-      <c r="L119" t="inlineStr">
-        <is>
-          <t>439/24</t>
-        </is>
-      </c>
-      <c r="M119" t="inlineStr">
-        <is>
-          <t>304(2)BNS@311BNS</t>
-        </is>
-      </c>
+      <c r="L119" t="inlineStr"/>
+      <c r="M119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -7170,16 +6298,8 @@
       <c r="I120" t="inlineStr"/>
       <c r="J120" t="inlineStr"/>
       <c r="K120" t="inlineStr"/>
-      <c r="L120" t="inlineStr">
-        <is>
-          <t>439/24</t>
-        </is>
-      </c>
-      <c r="M120" t="inlineStr">
-        <is>
-          <t>304(2)BNS@311BNS</t>
-        </is>
-      </c>
+      <c r="L120" t="inlineStr"/>
+      <c r="M120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -7235,16 +6355,8 @@
       </c>
       <c r="J121" t="inlineStr"/>
       <c r="K121" t="inlineStr"/>
-      <c r="L121" t="inlineStr">
-        <is>
-          <t>218/2024</t>
-        </is>
-      </c>
-      <c r="M121" t="inlineStr">
-        <is>
-          <t>126(2),296(b),118(i),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L121" t="inlineStr"/>
+      <c r="M121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -7297,16 +6409,8 @@
       </c>
       <c r="J122" t="inlineStr"/>
       <c r="K122" t="inlineStr"/>
-      <c r="L122" t="inlineStr">
-        <is>
-          <t>218/2024</t>
-        </is>
-      </c>
-      <c r="M122" t="inlineStr">
-        <is>
-          <t>126(2),296(b),118(i),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L122" t="inlineStr"/>
+      <c r="M122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -7357,16 +6461,8 @@
       </c>
       <c r="J123" t="inlineStr"/>
       <c r="K123" t="inlineStr"/>
-      <c r="L123" t="inlineStr">
-        <is>
-          <t>197/24</t>
-        </is>
-      </c>
-      <c r="M123" t="inlineStr">
-        <is>
-          <t>296(b),351(3)BNS&amp;4ofTNPHWAct</t>
-        </is>
-      </c>
+      <c r="L123" t="inlineStr"/>
+      <c r="M123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -7426,16 +6522,8 @@
       </c>
       <c r="J124" t="inlineStr"/>
       <c r="K124" t="inlineStr"/>
-      <c r="L124" t="inlineStr">
-        <is>
-          <t>197/24</t>
-        </is>
-      </c>
-      <c r="M124" t="inlineStr">
-        <is>
-          <t>296(b),351(3)BNS&amp;4ofTNPHWAct</t>
-        </is>
-      </c>
+      <c r="L124" t="inlineStr"/>
+      <c r="M124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -7487,16 +6575,8 @@
       </c>
       <c r="J125" t="inlineStr"/>
       <c r="K125" t="inlineStr"/>
-      <c r="L125" t="inlineStr">
-        <is>
-          <t>23/23</t>
-        </is>
-      </c>
-      <c r="M125" t="inlineStr">
-        <is>
-          <t>394IPC(nbw)</t>
-        </is>
-      </c>
+      <c r="L125" t="inlineStr"/>
+      <c r="M125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -7540,16 +6620,8 @@
       </c>
       <c r="J126" t="inlineStr"/>
       <c r="K126" t="inlineStr"/>
-      <c r="L126" t="inlineStr">
-        <is>
-          <t>184/24</t>
-        </is>
-      </c>
-      <c r="M126" t="inlineStr">
-        <is>
-          <t>296(b),115(2),351(2)</t>
-        </is>
-      </c>
+      <c r="L126" t="inlineStr"/>
+      <c r="M126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -7609,16 +6681,8 @@
       </c>
       <c r="J127" t="inlineStr"/>
       <c r="K127" t="inlineStr"/>
-      <c r="L127" t="inlineStr">
-        <is>
-          <t>219/2024</t>
-        </is>
-      </c>
-      <c r="M127" t="inlineStr">
-        <is>
-          <t>8(c)r/w20(b)(ii)(A)NDPSAct296(6),132,351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L127" t="inlineStr"/>
+      <c r="M127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -7671,16 +6735,8 @@
       </c>
       <c r="J128" t="inlineStr"/>
       <c r="K128" t="inlineStr"/>
-      <c r="L128" t="inlineStr">
-        <is>
-          <t>199/22</t>
-        </is>
-      </c>
-      <c r="M128" t="inlineStr">
-        <is>
-          <t>294(b),324,506(ii)IPC</t>
-        </is>
-      </c>
+      <c r="L128" t="inlineStr"/>
+      <c r="M128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -7738,16 +6794,8 @@
       </c>
       <c r="J129" t="inlineStr"/>
       <c r="K129" t="inlineStr"/>
-      <c r="L129" t="inlineStr">
-        <is>
-          <t>266/2024</t>
-        </is>
-      </c>
-      <c r="M129" t="inlineStr">
-        <is>
-          <t>:296(b),115(2),118(1)351(3)BNSActand4ofTNPHWAct</t>
-        </is>
-      </c>
+      <c r="L129" t="inlineStr"/>
+      <c r="M129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -7796,16 +6844,8 @@
       </c>
       <c r="J130" t="inlineStr"/>
       <c r="K130" t="inlineStr"/>
-      <c r="L130" t="inlineStr">
-        <is>
-          <t>267/2024</t>
-        </is>
-      </c>
-      <c r="M130" t="inlineStr">
-        <is>
-          <t>:303(2),BNSAct(RedSandTheft)</t>
-        </is>
-      </c>
+      <c r="L130" t="inlineStr"/>
+      <c r="M130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -7852,16 +6892,8 @@
       </c>
       <c r="J131" t="inlineStr"/>
       <c r="K131" t="inlineStr"/>
-      <c r="L131" t="inlineStr">
-        <is>
-          <t>267/2024</t>
-        </is>
-      </c>
-      <c r="M131" t="inlineStr">
-        <is>
-          <t>:303(2),BNSAct(RedSandTheft)</t>
-        </is>
-      </c>
+      <c r="L131" t="inlineStr"/>
+      <c r="M131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -7913,16 +6945,8 @@
       </c>
       <c r="J132" t="inlineStr"/>
       <c r="K132" t="inlineStr"/>
-      <c r="L132" t="inlineStr">
-        <is>
-          <t>267/2024</t>
-        </is>
-      </c>
-      <c r="M132" t="inlineStr">
-        <is>
-          <t>:303(2),BNSAct(RedSandTheft)</t>
-        </is>
-      </c>
+      <c r="L132" t="inlineStr"/>
+      <c r="M132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -7989,16 +7013,8 @@
       </c>
       <c r="J133" t="inlineStr"/>
       <c r="K133" t="inlineStr"/>
-      <c r="L133" t="inlineStr">
-        <is>
-          <t>267/2024</t>
-        </is>
-      </c>
-      <c r="M133" t="inlineStr">
-        <is>
-          <t>:303(2),BNSAct(RedSandTheft)</t>
-        </is>
-      </c>
+      <c r="L133" t="inlineStr"/>
+      <c r="M133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -8049,16 +7065,8 @@
       </c>
       <c r="J134" t="inlineStr"/>
       <c r="K134" t="inlineStr"/>
-      <c r="L134" t="inlineStr">
-        <is>
-          <t>88/2024</t>
-        </is>
-      </c>
-      <c r="M134" t="inlineStr">
-        <is>
-          <t>296(b),132,351(3)BNS8(c)r/w20(b)(ii)(A)NDPSAct1985</t>
-        </is>
-      </c>
+      <c r="L134" t="inlineStr"/>
+      <c r="M134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -8104,16 +7112,8 @@
       </c>
       <c r="J135" t="inlineStr"/>
       <c r="K135" t="inlineStr"/>
-      <c r="L135" t="inlineStr">
-        <is>
-          <t>85/24</t>
-        </is>
-      </c>
-      <c r="M135" t="inlineStr">
-        <is>
-          <t>.103(1)BNS</t>
-        </is>
-      </c>
+      <c r="L135" t="inlineStr"/>
+      <c r="M135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -8160,16 +7160,8 @@
       </c>
       <c r="J136" t="inlineStr"/>
       <c r="K136" t="inlineStr"/>
-      <c r="L136" t="inlineStr">
-        <is>
-          <t>270/24</t>
-        </is>
-      </c>
-      <c r="M136" t="inlineStr">
-        <is>
-          <t>.332(b),296(b),103(1),351(3)BNSAct</t>
-        </is>
-      </c>
+      <c r="L136" t="inlineStr"/>
+      <c r="M136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -8208,16 +7200,8 @@
       </c>
       <c r="J137" t="inlineStr"/>
       <c r="K137" t="inlineStr"/>
-      <c r="L137" t="inlineStr">
-        <is>
-          <t>236/2024</t>
-        </is>
-      </c>
-      <c r="M137" t="inlineStr">
-        <is>
-          <t>352,353(2)BNS</t>
-        </is>
-      </c>
+      <c r="L137" t="inlineStr"/>
+      <c r="M137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -8263,16 +7247,8 @@
       </c>
       <c r="J138" t="inlineStr"/>
       <c r="K138" t="inlineStr"/>
-      <c r="L138" t="inlineStr">
-        <is>
-          <t>223/24</t>
-        </is>
-      </c>
-      <c r="M138" t="inlineStr">
-        <is>
-          <t>126(2),296(b),308(2),118(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L138" t="inlineStr"/>
+      <c r="M138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -8318,16 +7294,8 @@
       </c>
       <c r="J139" t="inlineStr"/>
       <c r="K139" t="inlineStr"/>
-      <c r="L139" t="inlineStr">
-        <is>
-          <t>303/24</t>
-        </is>
-      </c>
-      <c r="M139" t="inlineStr">
-        <is>
-          <t>.126(2),296(b),308(4),351(3)-BNS</t>
-        </is>
-      </c>
+      <c r="L139" t="inlineStr"/>
+      <c r="M139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -8373,16 +7341,8 @@
       </c>
       <c r="J140" t="inlineStr"/>
       <c r="K140" t="inlineStr"/>
-      <c r="L140" t="inlineStr">
-        <is>
-          <t>297/24</t>
-        </is>
-      </c>
-      <c r="M140" t="inlineStr">
-        <is>
-          <t>-326(F)</t>
-        </is>
-      </c>
+      <c r="L140" t="inlineStr"/>
+      <c r="M140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -8428,16 +7388,8 @@
       </c>
       <c r="J141" t="inlineStr"/>
       <c r="K141" t="inlineStr"/>
-      <c r="L141" t="inlineStr">
-        <is>
-          <t>419/24</t>
-        </is>
-      </c>
-      <c r="M141" t="inlineStr">
-        <is>
-          <t>296(b),115(2),127(2),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L141" t="inlineStr"/>
+      <c r="M141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -8483,16 +7435,8 @@
       </c>
       <c r="J142" t="inlineStr"/>
       <c r="K142" t="inlineStr"/>
-      <c r="L142" t="inlineStr">
-        <is>
-          <t>419/24</t>
-        </is>
-      </c>
-      <c r="M142" t="inlineStr">
-        <is>
-          <t>296(b),115(2),127(2),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L142" t="inlineStr"/>
+      <c r="M142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -8542,16 +7486,8 @@
       </c>
       <c r="J143" t="inlineStr"/>
       <c r="K143" t="inlineStr"/>
-      <c r="L143" t="inlineStr">
-        <is>
-          <t>513/24</t>
-        </is>
-      </c>
-      <c r="M143" t="inlineStr">
-        <is>
-          <t>303(2)BNS</t>
-        </is>
-      </c>
+      <c r="L143" t="inlineStr"/>
+      <c r="M143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -8606,16 +7542,8 @@
       </c>
       <c r="J144" t="inlineStr"/>
       <c r="K144" t="inlineStr"/>
-      <c r="L144" t="inlineStr">
-        <is>
-          <t>106/24</t>
-        </is>
-      </c>
-      <c r="M144" t="inlineStr">
-        <is>
-          <t>296(b),118(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L144" t="inlineStr"/>
+      <c r="M144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -8693,14 +7621,10 @@
       <c r="K145" t="inlineStr"/>
       <c r="L145" t="inlineStr">
         <is>
-          <t>317/2024</t>
-        </is>
-      </c>
-      <c r="M145" t="inlineStr">
-        <is>
-          <t>:311,351(3)BNS</t>
-        </is>
-      </c>
+          <t>317/2024/3113513</t>
+        </is>
+      </c>
+      <c r="M145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -8777,16 +7701,8 @@
       </c>
       <c r="J146" t="inlineStr"/>
       <c r="K146" t="inlineStr"/>
-      <c r="L146" t="inlineStr">
-        <is>
-          <t>472/2024</t>
-        </is>
-      </c>
-      <c r="M146" t="inlineStr">
-        <is>
-          <t>.296(b),308(2),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L146" t="inlineStr"/>
+      <c r="M146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -8834,16 +7750,8 @@
       </c>
       <c r="J147" t="inlineStr"/>
       <c r="K147" t="inlineStr"/>
-      <c r="L147" t="inlineStr">
-        <is>
-          <t>272/24</t>
-        </is>
-      </c>
-      <c r="M147" t="inlineStr">
-        <is>
-          <t>.311,309(4)BNSAct</t>
-        </is>
-      </c>
+      <c r="L147" t="inlineStr"/>
+      <c r="M147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -8899,16 +7807,8 @@
       </c>
       <c r="J148" t="inlineStr"/>
       <c r="K148" t="inlineStr"/>
-      <c r="L148" t="inlineStr">
-        <is>
-          <t>272/24</t>
-        </is>
-      </c>
-      <c r="M148" t="inlineStr">
-        <is>
-          <t>.311,309(4)BNSAct</t>
-        </is>
-      </c>
+      <c r="L148" t="inlineStr"/>
+      <c r="M148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -8966,16 +7866,8 @@
       </c>
       <c r="J149" t="inlineStr"/>
       <c r="K149" t="inlineStr"/>
-      <c r="L149" t="inlineStr">
-        <is>
-          <t>272/24</t>
-        </is>
-      </c>
-      <c r="M149" t="inlineStr">
-        <is>
-          <t>.311,309(4)BNSAct</t>
-        </is>
-      </c>
+      <c r="L149" t="inlineStr"/>
+      <c r="M149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -9022,16 +7914,8 @@
       </c>
       <c r="J150" t="inlineStr"/>
       <c r="K150" t="inlineStr"/>
-      <c r="L150" t="inlineStr">
-        <is>
-          <t>162/2024</t>
-        </is>
-      </c>
-      <c r="M150" t="inlineStr">
-        <is>
-          <t>296(b),324(4),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L150" t="inlineStr"/>
+      <c r="M150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -9081,16 +7965,8 @@
       </c>
       <c r="J151" t="inlineStr"/>
       <c r="K151" t="inlineStr"/>
-      <c r="L151" t="inlineStr">
-        <is>
-          <t>282/2024</t>
-        </is>
-      </c>
-      <c r="M151" t="inlineStr">
-        <is>
-          <t>126(2),127(2),296(b),115(2),18(1),351(3),3(5)BNS3(1)(r),3(1)(va)</t>
-        </is>
-      </c>
+      <c r="L151" t="inlineStr"/>
+      <c r="M151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -9373,16 +8249,8 @@
       </c>
       <c r="J158" t="inlineStr"/>
       <c r="K158" t="inlineStr"/>
-      <c r="L158" t="inlineStr">
-        <is>
-          <t>265/24</t>
-        </is>
-      </c>
-      <c r="M158" t="inlineStr">
-        <is>
-          <t>296(b),115(2),351(3)BNS&amp;amp;4ofTNPWHAct</t>
-        </is>
-      </c>
+      <c r="L158" t="inlineStr"/>
+      <c r="M158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -9434,16 +8302,8 @@
       </c>
       <c r="J159" t="inlineStr"/>
       <c r="K159" t="inlineStr"/>
-      <c r="L159" t="inlineStr">
-        <is>
-          <t>123/24</t>
-        </is>
-      </c>
-      <c r="M159" t="inlineStr">
-        <is>
-          <t>.296(b),109(1),BNSAct</t>
-        </is>
-      </c>
+      <c r="L159" t="inlineStr"/>
+      <c r="M159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -9491,16 +8351,8 @@
       </c>
       <c r="J160" t="inlineStr"/>
       <c r="K160" t="inlineStr"/>
-      <c r="L160" t="inlineStr">
-        <is>
-          <t>123/24</t>
-        </is>
-      </c>
-      <c r="M160" t="inlineStr">
-        <is>
-          <t>.296(b),109(1),BNSAct</t>
-        </is>
-      </c>
+      <c r="L160" t="inlineStr"/>
+      <c r="M160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -9591,16 +8443,8 @@
       </c>
       <c r="J161" t="inlineStr"/>
       <c r="K161" t="inlineStr"/>
-      <c r="L161" t="inlineStr">
-        <is>
-          <t>123/24</t>
-        </is>
-      </c>
-      <c r="M161" t="inlineStr">
-        <is>
-          <t>.296(b),109(1),BNSAct</t>
-        </is>
-      </c>
+      <c r="L161" t="inlineStr"/>
+      <c r="M161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -9672,16 +8516,8 @@
       </c>
       <c r="J162" t="inlineStr"/>
       <c r="K162" t="inlineStr"/>
-      <c r="L162" t="inlineStr">
-        <is>
-          <t>155/22</t>
-        </is>
-      </c>
-      <c r="M162" t="inlineStr">
-        <is>
-          <t>:294(b),427,307,506(ii)IPC.&amp;4OfTNPHWAct.-mahilacourt-TUTSCNo.55/23</t>
-        </is>
-      </c>
+      <c r="L162" t="inlineStr"/>
+      <c r="M162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -9727,16 +8563,8 @@
       </c>
       <c r="J163" t="inlineStr"/>
       <c r="K163" t="inlineStr"/>
-      <c r="L163" t="inlineStr">
-        <is>
-          <t>514/24</t>
-        </is>
-      </c>
-      <c r="M163" t="inlineStr">
-        <is>
-          <t>296(b),118(1),109(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L163" t="inlineStr"/>
+      <c r="M163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -9782,16 +8610,8 @@
       </c>
       <c r="J164" t="inlineStr"/>
       <c r="K164" t="inlineStr"/>
-      <c r="L164" t="inlineStr">
-        <is>
-          <t>14/24</t>
-        </is>
-      </c>
-      <c r="M164" t="inlineStr">
-        <is>
-          <t>9mr/w10,PocsoAct329(4),351(2)BNS</t>
-        </is>
-      </c>
+      <c r="L164" t="inlineStr"/>
+      <c r="M164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -9952,16 +8772,8 @@
       </c>
       <c r="J167" t="inlineStr"/>
       <c r="K167" t="inlineStr"/>
-      <c r="L167" t="inlineStr">
-        <is>
-          <t>217/2024</t>
-        </is>
-      </c>
-      <c r="M167" t="inlineStr">
-        <is>
-          <t>126(2),296(b),115(2),118(1),351(iii)BNS</t>
-        </is>
-      </c>
+      <c r="L167" t="inlineStr"/>
+      <c r="M167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -10007,16 +8819,8 @@
       </c>
       <c r="J168" t="inlineStr"/>
       <c r="K168" t="inlineStr"/>
-      <c r="L168" t="inlineStr">
-        <is>
-          <t>217/2024</t>
-        </is>
-      </c>
-      <c r="M168" t="inlineStr">
-        <is>
-          <t>126(2),296(b),115(2),118(1),351(iii)BNS</t>
-        </is>
-      </c>
+      <c r="L168" t="inlineStr"/>
+      <c r="M168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -10064,16 +8868,8 @@
       </c>
       <c r="J169" t="inlineStr"/>
       <c r="K169" t="inlineStr"/>
-      <c r="L169" t="inlineStr">
-        <is>
-          <t>217/2024</t>
-        </is>
-      </c>
-      <c r="M169" t="inlineStr">
-        <is>
-          <t>126(2),296(b),115(2),118(1),351(iii)BNS</t>
-        </is>
-      </c>
+      <c r="L169" t="inlineStr"/>
+      <c r="M169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -10119,16 +8915,8 @@
       </c>
       <c r="J170" t="inlineStr"/>
       <c r="K170" t="inlineStr"/>
-      <c r="L170" t="inlineStr">
-        <is>
-          <t>217/2024</t>
-        </is>
-      </c>
-      <c r="M170" t="inlineStr">
-        <is>
-          <t>126(2),296(b),115(2),118(1),351(iii)BNS</t>
-        </is>
-      </c>
+      <c r="L170" t="inlineStr"/>
+      <c r="M170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -10181,16 +8969,8 @@
       </c>
       <c r="J171" t="inlineStr"/>
       <c r="K171" t="inlineStr"/>
-      <c r="L171" t="inlineStr">
-        <is>
-          <t>473/2024</t>
-        </is>
-      </c>
-      <c r="M171" t="inlineStr">
-        <is>
-          <t>.296(b),118(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L171" t="inlineStr"/>
+      <c r="M171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -10269,16 +9049,8 @@
       </c>
       <c r="J172" t="inlineStr"/>
       <c r="K172" t="inlineStr"/>
-      <c r="L172" t="inlineStr">
-        <is>
-          <t>473/2024</t>
-        </is>
-      </c>
-      <c r="M172" t="inlineStr">
-        <is>
-          <t>.296(b),118(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L172" t="inlineStr"/>
+      <c r="M172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -10332,16 +9104,8 @@
       </c>
       <c r="J173" t="inlineStr"/>
       <c r="K173" t="inlineStr"/>
-      <c r="L173" t="inlineStr">
-        <is>
-          <t>315/2024</t>
-        </is>
-      </c>
-      <c r="M173" t="inlineStr">
-        <is>
-          <t>:296(b),132,351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L173" t="inlineStr"/>
+      <c r="M173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -10424,16 +9188,8 @@
       </c>
       <c r="J174" t="inlineStr"/>
       <c r="K174" t="inlineStr"/>
-      <c r="L174" t="inlineStr">
-        <is>
-          <t>315/2024</t>
-        </is>
-      </c>
-      <c r="M174" t="inlineStr">
-        <is>
-          <t>:296(b),132,351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L174" t="inlineStr"/>
+      <c r="M174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -10519,16 +9275,8 @@
       </c>
       <c r="J175" t="inlineStr"/>
       <c r="K175" t="inlineStr"/>
-      <c r="L175" t="inlineStr">
-        <is>
-          <t>315/2024</t>
-        </is>
-      </c>
-      <c r="M175" t="inlineStr">
-        <is>
-          <t>:296(b),132,351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L175" t="inlineStr"/>
+      <c r="M175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -10574,16 +9322,8 @@
       </c>
       <c r="J176" t="inlineStr"/>
       <c r="K176" t="inlineStr"/>
-      <c r="L176" t="inlineStr">
-        <is>
-          <t>81/24</t>
-        </is>
-      </c>
-      <c r="M176" t="inlineStr">
-        <is>
-          <t>331(3),305BNS</t>
-        </is>
-      </c>
+      <c r="L176" t="inlineStr"/>
+      <c r="M176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -10631,16 +9371,8 @@
       </c>
       <c r="J177" t="inlineStr"/>
       <c r="K177" t="inlineStr"/>
-      <c r="L177" t="inlineStr">
-        <is>
-          <t>81/24</t>
-        </is>
-      </c>
-      <c r="M177" t="inlineStr">
-        <is>
-          <t>331(3),305BNS</t>
-        </is>
-      </c>
+      <c r="L177" t="inlineStr"/>
+      <c r="M177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -10694,16 +9426,8 @@
       </c>
       <c r="J178" t="inlineStr"/>
       <c r="K178" t="inlineStr"/>
-      <c r="L178" t="inlineStr">
-        <is>
-          <t>81/24</t>
-        </is>
-      </c>
-      <c r="M178" t="inlineStr">
-        <is>
-          <t>331(3),305BNS</t>
-        </is>
-      </c>
+      <c r="L178" t="inlineStr"/>
+      <c r="M178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -10754,16 +9478,8 @@
       </c>
       <c r="J179" t="inlineStr"/>
       <c r="K179" t="inlineStr"/>
-      <c r="L179" t="inlineStr">
-        <is>
-          <t>200/24</t>
-        </is>
-      </c>
-      <c r="M179" t="inlineStr">
-        <is>
-          <t>296(b),118(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L179" t="inlineStr"/>
+      <c r="M179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -10813,16 +9529,8 @@
       </c>
       <c r="J180" t="inlineStr"/>
       <c r="K180" t="inlineStr"/>
-      <c r="L180" t="inlineStr">
-        <is>
-          <t>320/24</t>
-        </is>
-      </c>
-      <c r="M180" t="inlineStr">
-        <is>
-          <t>:8©,r/w20(b),(ii),(B),25,29(1)NDPSACT</t>
-        </is>
-      </c>
+      <c r="L180" t="inlineStr"/>
+      <c r="M180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -10873,16 +9581,8 @@
       </c>
       <c r="J181" t="inlineStr"/>
       <c r="K181" t="inlineStr"/>
-      <c r="L181" t="inlineStr">
-        <is>
-          <t>320/24</t>
-        </is>
-      </c>
-      <c r="M181" t="inlineStr">
-        <is>
-          <t>:8©,r/w20(b),(ii),(B),25,29(1)NDPSACT</t>
-        </is>
-      </c>
+      <c r="L181" t="inlineStr"/>
+      <c r="M181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -10931,16 +9631,8 @@
       </c>
       <c r="J182" t="inlineStr"/>
       <c r="K182" t="inlineStr"/>
-      <c r="L182" t="inlineStr">
-        <is>
-          <t>320/24</t>
-        </is>
-      </c>
-      <c r="M182" t="inlineStr">
-        <is>
-          <t>:8©,r/w20(b),(ii),(B),25,29(1)NDPSACT</t>
-        </is>
-      </c>
+      <c r="L182" t="inlineStr"/>
+      <c r="M182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -10989,16 +9681,8 @@
       </c>
       <c r="J183" t="inlineStr"/>
       <c r="K183" t="inlineStr"/>
-      <c r="L183" t="inlineStr">
-        <is>
-          <t>320/24</t>
-        </is>
-      </c>
-      <c r="M183" t="inlineStr">
-        <is>
-          <t>:8©,r/w20(b),(ii),(B),25,29(1)NDPSACT</t>
-        </is>
-      </c>
+      <c r="L183" t="inlineStr"/>
+      <c r="M183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -11064,16 +9748,8 @@
       </c>
       <c r="J184" t="inlineStr"/>
       <c r="K184" t="inlineStr"/>
-      <c r="L184" t="inlineStr">
-        <is>
-          <t>171/24</t>
-        </is>
-      </c>
-      <c r="M184" t="inlineStr">
-        <is>
-          <t>296(b),79,351(3)-BNS</t>
-        </is>
-      </c>
+      <c r="L184" t="inlineStr"/>
+      <c r="M184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -11119,16 +9795,8 @@
       </c>
       <c r="J185" t="inlineStr"/>
       <c r="K185" t="inlineStr"/>
-      <c r="L185" t="inlineStr">
-        <is>
-          <t>296/24</t>
-        </is>
-      </c>
-      <c r="M185" t="inlineStr">
-        <is>
-          <t>30(2)BNS</t>
-        </is>
-      </c>
+      <c r="L185" t="inlineStr"/>
+      <c r="M185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -11174,16 +9842,8 @@
       </c>
       <c r="J186" t="inlineStr"/>
       <c r="K186" t="inlineStr"/>
-      <c r="L186" t="inlineStr">
-        <is>
-          <t>296/24</t>
-        </is>
-      </c>
-      <c r="M186" t="inlineStr">
-        <is>
-          <t>30(2)BNS</t>
-        </is>
-      </c>
+      <c r="L186" t="inlineStr"/>
+      <c r="M186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -11229,16 +9889,8 @@
       </c>
       <c r="J187" t="inlineStr"/>
       <c r="K187" t="inlineStr"/>
-      <c r="L187" t="inlineStr">
-        <is>
-          <t>476/2024</t>
-        </is>
-      </c>
-      <c r="M187" t="inlineStr">
-        <is>
-          <t>296(b),115(2),121(1),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L187" t="inlineStr"/>
+      <c r="M187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -11284,16 +9936,8 @@
       </c>
       <c r="J188" t="inlineStr"/>
       <c r="K188" t="inlineStr"/>
-      <c r="L188" t="inlineStr">
-        <is>
-          <t>475/2024</t>
-        </is>
-      </c>
-      <c r="M188" t="inlineStr">
-        <is>
-          <t>.-191(2),191(3),127(2),296(b),118(2),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L188" t="inlineStr"/>
+      <c r="M188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -11339,16 +9983,8 @@
       </c>
       <c r="J189" t="inlineStr"/>
       <c r="K189" t="inlineStr"/>
-      <c r="L189" t="inlineStr">
-        <is>
-          <t>475/2024</t>
-        </is>
-      </c>
-      <c r="M189" t="inlineStr">
-        <is>
-          <t>.-191(2),191(3),127(2),296(b),118(2),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L189" t="inlineStr"/>
+      <c r="M189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -11394,16 +10030,8 @@
       </c>
       <c r="J190" t="inlineStr"/>
       <c r="K190" t="inlineStr"/>
-      <c r="L190" t="inlineStr">
-        <is>
-          <t>477/2024</t>
-        </is>
-      </c>
-      <c r="M190" t="inlineStr">
-        <is>
-          <t>192,352,353(1)©(2)BNS</t>
-        </is>
-      </c>
+      <c r="L190" t="inlineStr"/>
+      <c r="M190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -11551,16 +10179,8 @@
       </c>
       <c r="J193" t="inlineStr"/>
       <c r="K193" t="inlineStr"/>
-      <c r="L193" t="inlineStr">
-        <is>
-          <t>46/24</t>
-        </is>
-      </c>
-      <c r="M193" t="inlineStr">
-        <is>
-          <t>341,294(b),323,324,307,506(ii)IPC</t>
-        </is>
-      </c>
+      <c r="L193" t="inlineStr"/>
+      <c r="M193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -11606,16 +10226,8 @@
       </c>
       <c r="J194" t="inlineStr"/>
       <c r="K194" t="inlineStr"/>
-      <c r="L194" t="inlineStr">
-        <is>
-          <t>48/24</t>
-        </is>
-      </c>
-      <c r="M194" t="inlineStr">
-        <is>
-          <t>279,337IPC</t>
-        </is>
-      </c>
+      <c r="L194" t="inlineStr"/>
+      <c r="M194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -11661,16 +10273,8 @@
       </c>
       <c r="J195" t="inlineStr"/>
       <c r="K195" t="inlineStr"/>
-      <c r="L195" t="inlineStr">
-        <is>
-          <t>192/24</t>
-        </is>
-      </c>
-      <c r="M195" t="inlineStr">
-        <is>
-          <t>331(3),305BNS</t>
-        </is>
-      </c>
+      <c r="L195" t="inlineStr"/>
+      <c r="M195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -11751,16 +10355,8 @@
       </c>
       <c r="J197" t="inlineStr"/>
       <c r="K197" t="inlineStr"/>
-      <c r="L197" t="inlineStr">
-        <is>
-          <t>518/24</t>
-        </is>
-      </c>
-      <c r="M197" t="inlineStr">
-        <is>
-          <t>126(2),296(b),308(5),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L197" t="inlineStr"/>
+      <c r="M197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -11806,16 +10402,8 @@
       </c>
       <c r="J198" t="inlineStr"/>
       <c r="K198" t="inlineStr"/>
-      <c r="L198" t="inlineStr">
-        <is>
-          <t>518/24</t>
-        </is>
-      </c>
-      <c r="M198" t="inlineStr">
-        <is>
-          <t>126(2),296(b),308(5),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L198" t="inlineStr"/>
+      <c r="M198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -11861,16 +10449,8 @@
       </c>
       <c r="J199" t="inlineStr"/>
       <c r="K199" t="inlineStr"/>
-      <c r="L199" t="inlineStr">
-        <is>
-          <t>518/24</t>
-        </is>
-      </c>
-      <c r="M199" t="inlineStr">
-        <is>
-          <t>126(2),296(b),308(5),351(3)BNS</t>
-        </is>
-      </c>
+      <c r="L199" t="inlineStr"/>
+      <c r="M199" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>